<commit_message>
- Finished Implementation of DataProvider class - Implemented Search test cases - Modified excel file path in config file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test-Data.xlsx
+++ b/src/test/resources/testdata/Test-Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,10 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Check-in</t>
+    <t>CheckIn</t>
   </si>
   <si>
-    <t>Check-out</t>
+    <t>CheckOut</t>
   </si>
   <si>
     <t>Alexandria</t>
@@ -980,21 +980,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="25.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,9 +1003,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1014,6 @@
       <c r="C2" s="2">
         <v>45944</v>
       </c>
-      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Switched the Before&After Methods to Before&After Suite and driver to static to make the test cases sequential using the same data - Added the test suite and tested classes in testng xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test-Data.xlsx
+++ b/src/test/resources/testdata/Test-Data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Search" sheetId="1" r:id="rId1"/>
+    <sheet name="Hotel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Location</t>
   </si>
@@ -39,6 +40,12 @@
   </si>
   <si>
     <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Tolip</t>
   </si>
 </sst>
 </file>
@@ -653,8 +660,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,24 +1004,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>45931</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>45944</v>
       </c>
     </row>
@@ -1019,4 +1029,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Changed Access modifier of the js executor in all classes - changed the reservation process implementation to apply ddt
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test-Data.xlsx
+++ b/src/test/resources/testdata/Test-Data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="Hotel" sheetId="2" r:id="rId2"/>
+    <sheet name="Reservation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Location</t>
   </si>
@@ -46,6 +47,15 @@
   </si>
   <si>
     <t>Tolip</t>
+  </si>
+  <si>
+    <t>Bed</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Queen</t>
   </si>
 </sst>
 </file>
@@ -660,8 +670,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,8 +1008,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1004,24 +1020,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>45931</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>45944</v>
       </c>
     </row>
@@ -1043,12 +1059,12 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1056,4 +1072,37 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Added one extra sheet in TestData excel file - Modified date picking to be data-driven
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test-Data.xlsx
+++ b/src/test/resources/testdata/Test-Data.xlsx
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1035,10 +1035,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="5">
-        <v>45931</v>
+        <v>46023</v>
       </c>
       <c r="C2" s="5">
-        <v>45944</v>
+        <v>46036</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1080,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>